<commit_message>
rebuilding site Mon 05 Oct 2020 12:22:49 PM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/bendingData.xlsx
+++ b/engineering/courses/mae101/docs/bendingData.xlsx
@@ -284,7 +284,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -383,11 +383,11 @@
   </sheetPr>
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.99"/>
@@ -533,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="13" t="n">
         <v>2.5</v>
       </c>
@@ -541,7 +541,7 @@
         <v>31.75</v>
       </c>
       <c r="D8" s="11" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="14"/>
@@ -559,7 +559,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="12"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="13" t="n">
         <v>3.5</v>
       </c>
@@ -567,7 +567,7 @@
         <v>31.5625</v>
       </c>
       <c r="D9" s="11" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="15"/>
@@ -585,7 +585,7 @@
       <c r="N9" s="15"/>
       <c r="O9" s="12"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="13" t="n">
         <v>4.5</v>
       </c>
@@ -593,7 +593,7 @@
         <v>31.1875</v>
       </c>
       <c r="D10" s="11" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="15"/>
@@ -611,7 +611,7 @@
       <c r="N10" s="15"/>
       <c r="O10" s="12"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="13" t="n">
         <v>5.5</v>
       </c>
@@ -619,7 +619,7 @@
         <v>30.875</v>
       </c>
       <c r="D11" s="11" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="15"/>
@@ -637,7 +637,7 @@
       <c r="N11" s="15"/>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="13" t="n">
         <v>6.5</v>
       </c>
@@ -645,7 +645,7 @@
         <v>30.6875</v>
       </c>
       <c r="D12" s="11" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="15"/>
@@ -663,7 +663,7 @@
       <c r="N12" s="15"/>
       <c r="O12" s="12"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13" t="n">
         <v>7.5</v>
       </c>
@@ -671,7 +671,7 @@
         <v>30.3125</v>
       </c>
       <c r="D13" s="11" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="15"/>
@@ -683,7 +683,7 @@
       <c r="N13" s="15"/>
       <c r="O13" s="12"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="n">
         <v>8.5</v>
       </c>
@@ -691,7 +691,7 @@
         <v>30.1875</v>
       </c>
       <c r="D14" s="11" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="15"/>
@@ -791,7 +791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="13" t="n">
         <v>2.5</v>
       </c>
@@ -799,7 +799,7 @@
         <v>32.875</v>
       </c>
       <c r="D19" s="11" t="n">
-        <v>32.87</v>
+        <v>33</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="14"/>
@@ -811,13 +811,13 @@
         <v>30.06</v>
       </c>
       <c r="L19" s="11" t="n">
-        <v>30</v>
+        <v>30.07</v>
       </c>
       <c r="M19" s="11"/>
       <c r="N19" s="14"/>
       <c r="O19" s="12"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="13" t="n">
         <v>3.5</v>
       </c>
@@ -825,7 +825,7 @@
         <v>32.84375</v>
       </c>
       <c r="D20" s="11" t="n">
-        <v>32.87</v>
+        <v>33</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="15"/>
@@ -837,13 +837,13 @@
         <v>30.06</v>
       </c>
       <c r="L20" s="11" t="n">
-        <v>30</v>
+        <v>30.07</v>
       </c>
       <c r="M20" s="11"/>
       <c r="N20" s="15"/>
       <c r="O20" s="12"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="13" t="n">
         <v>4.5</v>
       </c>
@@ -851,7 +851,7 @@
         <v>32.78125</v>
       </c>
       <c r="D21" s="11" t="n">
-        <v>32.87</v>
+        <v>33</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="15"/>
@@ -863,13 +863,13 @@
         <v>29.9</v>
       </c>
       <c r="L21" s="11" t="n">
-        <v>30</v>
+        <v>30.07</v>
       </c>
       <c r="M21" s="11"/>
       <c r="N21" s="15"/>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="n">
         <v>5.5</v>
       </c>
@@ -877,7 +877,7 @@
         <v>32.75</v>
       </c>
       <c r="D22" s="11" t="n">
-        <v>32.87</v>
+        <v>33</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="15"/>
@@ -889,13 +889,13 @@
         <v>29.87</v>
       </c>
       <c r="L22" s="11" t="n">
-        <v>30</v>
+        <v>30.07</v>
       </c>
       <c r="M22" s="11"/>
       <c r="N22" s="15"/>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="13" t="n">
         <v>6.5</v>
       </c>
@@ -903,7 +903,7 @@
         <v>32.6875</v>
       </c>
       <c r="D23" s="11" t="n">
-        <v>32.87</v>
+        <v>33</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="15"/>
@@ -915,13 +915,13 @@
         <v>29.69</v>
       </c>
       <c r="L23" s="11" t="n">
-        <v>30</v>
+        <v>30.07</v>
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="15"/>
       <c r="O23" s="12"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="n">
         <v>7.5</v>
       </c>
@@ -929,7 +929,7 @@
         <v>32.71875</v>
       </c>
       <c r="D24" s="11" t="n">
-        <v>32.87</v>
+        <v>33</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="15"/>
@@ -941,7 +941,7 @@
       <c r="N24" s="15"/>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="13" t="n">
         <v>8.5</v>
       </c>
@@ -949,7 +949,7 @@
         <v>32.625</v>
       </c>
       <c r="D25" s="11" t="n">
-        <v>32.87</v>
+        <v>33</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="15"/>

</xml_diff>

<commit_message>
rebuilding site Thu 15 Oct 2020 07:23:26 AM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/bendingData.xlsx
+++ b/engineering/courses/mae101/docs/bendingData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
   <si>
     <t xml:space="preserve">Bending Of Beam Raw Data</t>
   </si>
@@ -95,6 +95,12 @@
     <t xml:space="preserve">RAW Data 3</t>
   </si>
   <si>
+    <t xml:space="preserve">RAW Data 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluminum beam (Flat side on Support)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Width (w) = 1.509 in
 Length (L) = 35.875 in
 Thickness (t) = 0.255 in
@@ -102,21 +108,225 @@
 	Elasticity (E) = 1.8*106 psi	</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Length </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= 31.25 inch, P= load, </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 1.007 inch, </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">thickness </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= 0.130 inch, </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">E </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= 10 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">psi   </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Load(lbs.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experimental deflection (inch)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluminum beam (short side on Support)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Width (w) = 0.255 in
 Length (L) = 35.875 in
 Thickness (t) = 1.509 in
 Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
 Elasticity (E) = 1.8*106 psi	</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Length </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= 35 inch, P= load, </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.130 inch, </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">thickness</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 1.007 inch, </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">E </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= 10 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> psi  </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -162,6 +372,35 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -177,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -241,6 +480,55 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -267,7 +555,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -304,36 +592,52 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -352,8 +656,64 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -383,11 +743,11 @@
   </sheetPr>
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O44" activeCellId="0" sqref="O44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.99"/>
@@ -395,6 +755,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.29"/>
   </cols>
@@ -495,7 +857,7 @@
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
@@ -511,7 +873,7 @@
       <c r="F7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="9" t="s">
@@ -529,12 +891,12 @@
       <c r="N7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="O7" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="13" t="n">
+      <c r="B8" s="11" t="n">
         <v>2.5</v>
       </c>
       <c r="C8" s="11" t="n">
@@ -544,9 +906,9 @@
         <v>32</v>
       </c>
       <c r="E8" s="11"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="12"/>
-      <c r="J8" s="13" t="n">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="J8" s="11" t="n">
         <v>2</v>
       </c>
       <c r="K8" s="11" t="n">
@@ -556,11 +918,11 @@
         <v>28</v>
       </c>
       <c r="M8" s="11"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="12"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="13" t="n">
+      <c r="B9" s="11" t="n">
         <v>3.5</v>
       </c>
       <c r="C9" s="11" t="n">
@@ -570,9 +932,9 @@
         <v>32</v>
       </c>
       <c r="E9" s="11"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="12"/>
-      <c r="J9" s="13" t="n">
+      <c r="F9" s="12"/>
+      <c r="G9" s="9"/>
+      <c r="J9" s="11" t="n">
         <v>4</v>
       </c>
       <c r="K9" s="11" t="n">
@@ -582,11 +944,11 @@
         <v>28</v>
       </c>
       <c r="M9" s="11"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="13" t="n">
+      <c r="B10" s="11" t="n">
         <v>4.5</v>
       </c>
       <c r="C10" s="11" t="n">
@@ -596,9 +958,9 @@
         <v>32</v>
       </c>
       <c r="E10" s="11"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="12"/>
-      <c r="J10" s="13" t="n">
+      <c r="F10" s="12"/>
+      <c r="G10" s="9"/>
+      <c r="J10" s="11" t="n">
         <v>6</v>
       </c>
       <c r="K10" s="11" t="n">
@@ -608,11 +970,11 @@
         <v>28</v>
       </c>
       <c r="M10" s="11"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="13" t="n">
+      <c r="B11" s="11" t="n">
         <v>5.5</v>
       </c>
       <c r="C11" s="11" t="n">
@@ -622,9 +984,9 @@
         <v>32</v>
       </c>
       <c r="E11" s="11"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="12"/>
-      <c r="J11" s="13" t="n">
+      <c r="F11" s="12"/>
+      <c r="G11" s="9"/>
+      <c r="J11" s="11" t="n">
         <v>8</v>
       </c>
       <c r="K11" s="11" t="n">
@@ -634,11 +996,11 @@
         <v>28</v>
       </c>
       <c r="M11" s="11"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="13" t="n">
+      <c r="B12" s="11" t="n">
         <v>6.5</v>
       </c>
       <c r="C12" s="11" t="n">
@@ -648,9 +1010,9 @@
         <v>32</v>
       </c>
       <c r="E12" s="11"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="12"/>
-      <c r="J12" s="13" t="n">
+      <c r="F12" s="12"/>
+      <c r="G12" s="9"/>
+      <c r="J12" s="11" t="n">
         <v>10</v>
       </c>
       <c r="K12" s="11" t="n">
@@ -660,11 +1022,11 @@
         <v>28</v>
       </c>
       <c r="M12" s="11"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="13" t="n">
+      <c r="B13" s="11" t="n">
         <v>7.5</v>
       </c>
       <c r="C13" s="11" t="n">
@@ -674,17 +1036,17 @@
         <v>32</v>
       </c>
       <c r="E13" s="11"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="9"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="12"/>
+      <c r="O13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="13" t="n">
+      <c r="B14" s="11" t="n">
         <v>8.5</v>
       </c>
       <c r="C14" s="11" t="n">
@@ -694,46 +1056,46 @@
         <v>32</v>
       </c>
       <c r="E14" s="11"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="9"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
       <c r="N14" s="15"/>
-      <c r="O14" s="12"/>
+      <c r="O14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="9"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="12"/>
-      <c r="J15" s="9"/>
+      <c r="G15" s="16"/>
+      <c r="J15" s="17"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
-      <c r="O15" s="12"/>
+      <c r="O15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="J16" s="16" t="s">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="J16" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="7" t="s">
@@ -753,23 +1115,23 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="16" t="s">
         <v>17</v>
       </c>
       <c r="J18" s="9" t="s">
@@ -787,7 +1149,7 @@
       <c r="N18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="O18" s="12" t="s">
+      <c r="O18" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -795,16 +1157,16 @@
       <c r="B19" s="13" t="n">
         <v>2.5</v>
       </c>
-      <c r="C19" s="11" t="n">
+      <c r="C19" s="14" t="n">
         <v>32.875</v>
       </c>
-      <c r="D19" s="11" t="n">
+      <c r="D19" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="12"/>
-      <c r="J19" s="13" t="n">
+      <c r="E19" s="14"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="16"/>
+      <c r="J19" s="11" t="n">
         <v>2</v>
       </c>
       <c r="K19" s="11" t="n">
@@ -814,23 +1176,23 @@
         <v>30.07</v>
       </c>
       <c r="M19" s="11"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="12"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="13" t="n">
         <v>3.5</v>
       </c>
-      <c r="C20" s="11" t="n">
+      <c r="C20" s="14" t="n">
         <v>32.84375</v>
       </c>
-      <c r="D20" s="11" t="n">
+      <c r="D20" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="E20" s="11"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="12"/>
-      <c r="J20" s="13" t="n">
+      <c r="G20" s="16"/>
+      <c r="J20" s="11" t="n">
         <v>4</v>
       </c>
       <c r="K20" s="11" t="n">
@@ -840,23 +1202,23 @@
         <v>30.07</v>
       </c>
       <c r="M20" s="11"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="13" t="n">
         <v>4.5</v>
       </c>
-      <c r="C21" s="11" t="n">
+      <c r="C21" s="14" t="n">
         <v>32.78125</v>
       </c>
-      <c r="D21" s="11" t="n">
+      <c r="D21" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="E21" s="11"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="12"/>
-      <c r="J21" s="13" t="n">
+      <c r="G21" s="16"/>
+      <c r="J21" s="11" t="n">
         <v>6</v>
       </c>
       <c r="K21" s="11" t="n">
@@ -866,23 +1228,23 @@
         <v>30.07</v>
       </c>
       <c r="M21" s="11"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="n">
         <v>5.5</v>
       </c>
-      <c r="C22" s="11" t="n">
+      <c r="C22" s="14" t="n">
         <v>32.75</v>
       </c>
-      <c r="D22" s="11" t="n">
+      <c r="D22" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="E22" s="11"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="12"/>
-      <c r="J22" s="13" t="n">
+      <c r="G22" s="16"/>
+      <c r="J22" s="11" t="n">
         <v>8</v>
       </c>
       <c r="K22" s="11" t="n">
@@ -892,23 +1254,23 @@
         <v>30.07</v>
       </c>
       <c r="M22" s="11"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="13" t="n">
         <v>6.5</v>
       </c>
-      <c r="C23" s="11" t="n">
+      <c r="C23" s="14" t="n">
         <v>32.6875</v>
       </c>
-      <c r="D23" s="11" t="n">
+      <c r="D23" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="E23" s="11"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="15"/>
-      <c r="G23" s="12"/>
-      <c r="J23" s="13" t="n">
+      <c r="G23" s="16"/>
+      <c r="J23" s="11" t="n">
         <v>10</v>
       </c>
       <c r="K23" s="11" t="n">
@@ -918,68 +1280,68 @@
         <v>30.07</v>
       </c>
       <c r="M23" s="11"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="n">
         <v>7.5</v>
       </c>
-      <c r="C24" s="11" t="n">
+      <c r="C24" s="14" t="n">
         <v>32.71875</v>
       </c>
-      <c r="D24" s="11" t="n">
+      <c r="D24" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="15"/>
-      <c r="G24" s="12"/>
+      <c r="G24" s="16"/>
       <c r="J24" s="13"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
       <c r="N24" s="15"/>
-      <c r="O24" s="12"/>
+      <c r="O24" s="16"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="13" t="n">
         <v>8.5</v>
       </c>
-      <c r="C25" s="11" t="n">
+      <c r="C25" s="14" t="n">
         <v>32.625</v>
       </c>
-      <c r="D25" s="11" t="n">
+      <c r="D25" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="E25" s="11"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="15"/>
-      <c r="G25" s="12"/>
+      <c r="G25" s="16"/>
       <c r="J25" s="13"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
       <c r="N25" s="15"/>
-      <c r="O25" s="12"/>
+      <c r="O25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="19"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="23"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20"/>
+      <c r="A27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20"/>
+      <c r="A28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
@@ -990,6 +1352,14 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
+      <c r="J29" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="25"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="6" t="s">
@@ -1000,18 +1370,34 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
+      <c r="J30" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
     </row>
     <row r="31" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J31" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
         <v>7</v>
       </c>
@@ -1027,12 +1413,20 @@
       <c r="F32" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="13" t="n">
+      <c r="J32" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" s="30"/>
+      <c r="O32" s="31"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="11" t="n">
         <v>2.5</v>
       </c>
       <c r="C33" s="11" t="n">
@@ -1042,12 +1436,20 @@
         <v>3.316</v>
       </c>
       <c r="E33" s="11"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="12"/>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="21"/>
-      <c r="B34" s="13" t="n">
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="J33" s="9" t="n">
+        <v>2.465</v>
+      </c>
+      <c r="K33" s="11" t="n">
+        <v>0.255</v>
+      </c>
+      <c r="L33" s="11"/>
+      <c r="O33" s="31"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="32"/>
+      <c r="B34" s="11" t="n">
         <v>3.5</v>
       </c>
       <c r="C34" s="11" t="n">
@@ -1057,11 +1459,19 @@
         <v>3.316</v>
       </c>
       <c r="E34" s="11"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="12"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="13" t="n">
+      <c r="F34" s="12"/>
+      <c r="G34" s="9"/>
+      <c r="J34" s="9" t="n">
+        <v>4.465</v>
+      </c>
+      <c r="K34" s="11" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L34" s="11"/>
+      <c r="O34" s="31"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="11" t="n">
         <v>4.5</v>
       </c>
       <c r="C35" s="11" t="n">
@@ -1071,11 +1481,19 @@
         <v>3.316</v>
       </c>
       <c r="E35" s="11"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="12"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="13" t="n">
+      <c r="F35" s="12"/>
+      <c r="G35" s="9"/>
+      <c r="J35" s="9" t="n">
+        <v>6.465</v>
+      </c>
+      <c r="K35" s="11" t="n">
+        <v>1.755</v>
+      </c>
+      <c r="L35" s="11"/>
+      <c r="O35" s="31"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="11" t="n">
         <v>5.5</v>
       </c>
       <c r="C36" s="11" t="n">
@@ -1085,11 +1503,19 @@
         <v>3.316</v>
       </c>
       <c r="E36" s="11"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="12"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="13" t="n">
+      <c r="F36" s="12"/>
+      <c r="G36" s="9"/>
+      <c r="J36" s="9" t="n">
+        <v>8.465</v>
+      </c>
+      <c r="K36" s="11" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="L36" s="11"/>
+      <c r="O36" s="31"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="11" t="n">
         <v>6.5</v>
       </c>
       <c r="C37" s="11" t="n">
@@ -1099,38 +1525,64 @@
         <v>3.316</v>
       </c>
       <c r="E37" s="11"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="12"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="12"/>
+      <c r="G37" s="9"/>
+      <c r="J37" s="9" t="n">
+        <v>10.465</v>
+      </c>
+      <c r="K37" s="11" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="L37" s="11"/>
+      <c r="O37" s="31"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="13"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
       <c r="F38" s="15"/>
-      <c r="G38" s="12"/>
+      <c r="G38" s="16"/>
+      <c r="J38" s="33"/>
+      <c r="O38" s="31"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="J39" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
     </row>
     <row r="40" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J40" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="K40" s="34"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="34"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="9" t="s">
         <v>7</v>
       </c>
@@ -1146,12 +1598,20 @@
       <c r="F41" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="G41" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="13" t="n">
+      <c r="J41" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="L41" s="37"/>
+      <c r="O41" s="31"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="11" t="n">
         <v>2.5</v>
       </c>
       <c r="C42" s="11" t="n">
@@ -1161,11 +1621,19 @@
         <v>2.2</v>
       </c>
       <c r="E42" s="11"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="12"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="13" t="n">
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="J42" s="9" t="n">
+        <v>2.465</v>
+      </c>
+      <c r="K42" s="11" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="L42" s="11"/>
+      <c r="O42" s="31"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="11" t="n">
         <v>3.5</v>
       </c>
       <c r="C43" s="11" t="n">
@@ -1175,11 +1643,19 @@
         <v>2.2</v>
       </c>
       <c r="E43" s="11"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="12"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="13" t="n">
+      <c r="F43" s="12"/>
+      <c r="G43" s="9"/>
+      <c r="J43" s="9" t="n">
+        <v>4.465</v>
+      </c>
+      <c r="K43" s="11" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L43" s="11"/>
+      <c r="O43" s="31"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="11" t="n">
         <v>4.5</v>
       </c>
       <c r="C44" s="11" t="n">
@@ -1189,11 +1665,19 @@
         <v>2.2</v>
       </c>
       <c r="E44" s="11"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="12"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="13" t="n">
+      <c r="F44" s="12"/>
+      <c r="G44" s="9"/>
+      <c r="J44" s="9" t="n">
+        <v>6.465</v>
+      </c>
+      <c r="K44" s="11" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L44" s="11"/>
+      <c r="O44" s="31"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="11" t="n">
         <v>5.5</v>
       </c>
       <c r="C45" s="11" t="n">
@@ -1203,11 +1687,19 @@
         <v>2.2</v>
       </c>
       <c r="E45" s="11"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="12"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="13" t="n">
+      <c r="F45" s="12"/>
+      <c r="G45" s="9"/>
+      <c r="J45" s="9" t="n">
+        <v>8.465</v>
+      </c>
+      <c r="K45" s="11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L45" s="11"/>
+      <c r="O45" s="31"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="11" t="n">
         <v>6.5</v>
       </c>
       <c r="C46" s="11" t="n">
@@ -1217,110 +1709,120 @@
         <v>2.2</v>
       </c>
       <c r="E46" s="11"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="9"/>
+      <c r="J46" s="9" t="n">
+        <v>10.465</v>
+      </c>
+      <c r="K46" s="11" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="L46" s="11"/>
+      <c r="M46" s="38"/>
+      <c r="N46" s="38"/>
+      <c r="O46" s="39"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="13"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
       <c r="F47" s="15"/>
-      <c r="G47" s="12"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="13"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
       <c r="F48" s="15"/>
-      <c r="G48" s="12"/>
+      <c r="G48" s="16"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="19"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="23"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="22"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
     </row>
     <row r="56" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="15"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="11"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="14"/>
       <c r="G57" s="15"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="20"/>
       <c r="G58" s="15"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
       <c r="F63" s="15"/>
       <c r="G63" s="15"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
       <c r="F64" s="15"/>
       <c r="G64" s="15"/>
     </row>
@@ -1349,82 +1851,82 @@
       <c r="G67" s="15"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="22"/>
-      <c r="G68" s="22"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="40"/>
+      <c r="D68" s="40"/>
+      <c r="E68" s="40"/>
+      <c r="F68" s="40"/>
+      <c r="G68" s="40"/>
     </row>
     <row r="69" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="23"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="23"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="23"/>
-      <c r="G69" s="23"/>
+      <c r="B69" s="41"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="41"/>
+      <c r="G69" s="41"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="15"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="11"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="14"/>
       <c r="G70" s="15"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="20"/>
       <c r="G71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
       <c r="F76" s="15"/>
       <c r="G76" s="15"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
     </row>
@@ -1437,7 +1939,7 @@
       <c r="G78" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="32">
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="B5:G5"/>
@@ -1449,10 +1951,25 @@
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="J17:O17"/>
     <mergeCell ref="B29:G29"/>
+    <mergeCell ref="J29:O29"/>
     <mergeCell ref="B30:G30"/>
+    <mergeCell ref="J30:O30"/>
     <mergeCell ref="B31:G31"/>
+    <mergeCell ref="J31:O31"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
     <mergeCell ref="B39:G39"/>
+    <mergeCell ref="J39:O39"/>
     <mergeCell ref="B40:G40"/>
+    <mergeCell ref="J40:O40"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="K46:L46"/>
     <mergeCell ref="B55:G55"/>
     <mergeCell ref="B68:G68"/>
   </mergeCells>

</xml_diff>

<commit_message>
rebuilding site Thu 15 Oct 2020 07:34:49 AM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/bendingData.xlsx
+++ b/engineering/courses/mae101/docs/bendingData.xlsx
@@ -37,18 +37,95 @@
     <t xml:space="preserve">Case 1: Wood beam - flat side on support</t>
   </si>
   <si>
-    <t xml:space="preserve">Width (w) = 1.427 in
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Width (w) = 1.427 in
 Length (L) = 35.875 in
 Thickness (t) = 0.273 in
 	Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-	Elasticity (E) = 1.8*106 psi	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Width (w) = 1.54 in
+	Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> psi	</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Width (w) = 1.54 in
 Length (L) = 36 in
 Thickness (t) = 0.22 in
 	Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-	Elasticity (E) = 1.8*10^6 psi	</t>
+	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> psi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">	</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Weight (lb)</t>
@@ -72,18 +149,92 @@
     <t xml:space="preserve">Case 2: Wood beam - thin side on support</t>
   </si>
   <si>
-    <t xml:space="preserve">Width (w) = 0.273 in
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Width (w) = 0.273 in
 Length (L) = 35.875 in
 Thickness (t) = 1.427 in
 Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-Elasticity (E) = 1.8*10^6 psi	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Width (w) = 0.22 in
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> psi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Width (w) = 0.22 in
 Length (L) = 36 in
 Thickness (t) = 1.54 in
 Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-Elasticity (E) = 1.8*10^6 psi	</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> psi</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Experimental ∆h (in)</t>
@@ -101,11 +252,58 @@
     <t xml:space="preserve">Aluminum beam (Flat side on Support)</t>
   </si>
   <si>
-    <t xml:space="preserve">Width (w) = 1.509 in
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Width (w) = 1.509 in
 Length (L) = 35.875 in
 Thickness (t) = 0.255 in
 	Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-	Elasticity (E) = 1.8*106 psi	</t>
+	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> psi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">	</t>
+    </r>
   </si>
   <si>
     <r>
@@ -115,6 +313,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Length </t>
     </r>
@@ -124,6 +323,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= 31.25 inch, P= load, </t>
     </r>
@@ -134,6 +334,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Width</t>
     </r>
@@ -143,6 +344,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> = 1.007 inch, </t>
     </r>
@@ -153,6 +355,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">thickness </t>
     </r>
@@ -162,6 +365,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= 0.130 inch, </t>
     </r>
@@ -172,6 +376,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">E </t>
     </r>
@@ -181,6 +386,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= 10 x 10</t>
     </r>
@@ -191,6 +397,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6 </t>
     </r>
@@ -200,6 +407,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">psi   </t>
     </r>
@@ -214,11 +422,58 @@
     <t xml:space="preserve">Aluminum beam (short side on Support)</t>
   </si>
   <si>
-    <t xml:space="preserve">Width (w) = 0.255 in
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Width (w) = 0.255 in
 Length (L) = 35.875 in
 Thickness (t) = 1.509 in
 Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-Elasticity (E) = 1.8*106 psi	</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> psi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">	</t>
+    </r>
   </si>
   <si>
     <r>
@@ -228,6 +483,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Length </t>
     </r>
@@ -237,6 +493,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= 35 inch, P= load, </t>
     </r>
@@ -247,6 +504,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Width</t>
     </r>
@@ -256,6 +514,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> = 0.130 inch, </t>
     </r>
@@ -266,6 +525,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">thickness</t>
     </r>
@@ -275,6 +535,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> = 1.007 inch, </t>
     </r>
@@ -285,6 +546,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">E </t>
     </r>
@@ -294,6 +556,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= 10 x 10</t>
     </r>
@@ -304,6 +567,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6</t>
     </r>
@@ -313,6 +577,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> psi  </t>
     </r>
@@ -326,7 +591,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -366,6 +631,27 @@
       <charset val="1"/>
     </font>
     <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -378,12 +664,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -391,6 +679,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -596,7 +885,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -632,7 +921,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -652,7 +941,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -664,7 +953,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -684,7 +973,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -692,19 +981,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -743,11 +1032,11 @@
   </sheetPr>
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O44" activeCellId="0" sqref="O44"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F53" activeCellId="0" sqref="F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.99"/>
@@ -755,8 +1044,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.29"/>
   </cols>

</xml_diff>

<commit_message>
rebuilding site Fri 16 Oct 2020 10:55:31 AM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/bendingData.xlsx
+++ b/engineering/courses/mae101/docs/bendingData.xlsx
@@ -48,7 +48,7 @@
       <t xml:space="preserve">Width (w) = 1.427 in
 Length (L) = 35.875 in
 Thickness (t) = 0.273 in
-	Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
+	Inertia (I) = (w^3*t) ∕ 12   in^4
 	Elasticity (E) = 2*10</t>
     </r>
     <r>
@@ -85,46 +85,29 @@
       <t xml:space="preserve">Width (w) = 1.54 in
 Length (L) = 36 in
 Thickness (t) = 0.22 in
-	Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-	</t>
-    </r>
-    <r>
-      <rPr>
+	Inertia (I) = (w^3*t) ∕ 12    in^4
+	Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Elasticity (E) = 2*10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> psi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">	</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> psi	</t>
     </r>
   </si>
   <si>
@@ -160,34 +143,27 @@
       <t xml:space="preserve">Width (w) = 0.273 in
 Length (L) = 35.875 in
 Thickness (t) = 1.427 in
-Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-</t>
-    </r>
-    <r>
-      <rPr>
+Inertia (I) = (w^3*t) ∕ 12    in^4
+Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Elasticity (E) = 2*10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> psi</t>
     </r>
@@ -204,34 +180,27 @@
       <t xml:space="preserve">Width (w) = 0.22 in
 Length (L) = 36 in
 Thickness (t) = 1.54 in
-Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-</t>
-    </r>
-    <r>
-      <rPr>
+Inertia (I) = (w^3*t) ∕ 12    in^4
+Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Elasticity (E) = 2*10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> psi</t>
     </r>
@@ -263,46 +232,29 @@
       <t xml:space="preserve">Width (w) = 1.509 in
 Length (L) = 35.875 in
 Thickness (t) = 0.255 in
-	Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-	</t>
-    </r>
-    <r>
-      <rPr>
+	Inertia (I) = (w^3*t) ∕ 12    in^4
+	Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Elasticity (E) = 2*10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> psi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">	</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> psi	</t>
     </r>
   </si>
   <si>
@@ -434,45 +386,28 @@
 Length (L) = 35.875 in
 Thickness (t) = 1.509 in
 Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
-</t>
-    </r>
-    <r>
-      <rPr>
+Elasticity (E) = 2*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Elasticity (E) = 2*10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> psi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">	</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> psi	</t>
     </r>
   </si>
   <si>
@@ -591,7 +526,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -637,19 +572,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -885,7 +807,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -921,7 +843,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -941,7 +863,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -953,7 +875,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -973,7 +895,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -981,19 +903,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1032,11 +954,11 @@
   </sheetPr>
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F53" activeCellId="0" sqref="F53"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.99"/>
@@ -1045,7 +967,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.29"/>
   </cols>

</xml_diff>